<commit_message>
Feat: Update PR/PO/SR flow and add Status tracking features
</commit_message>
<xml_diff>
--- a/public/template.xlsx
+++ b/public/template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SupplyEase\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A7AF604-E15C-43B4-9313-4F37740E5966}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F5C1D3A-8481-4094-AA7E-ED58E2E2AF5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{3B32CD19-E252-4F93-8F09-25E85353E804}"/>
   </bookViews>
@@ -34,10 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>PR_No</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Item</t>
   </si>
@@ -46,13 +43,40 @@
   </si>
   <si>
     <t>Budget</t>
+  </si>
+  <si>
+    <t>A欄 (必填)</t>
+  </si>
+  <si>
+    <t>B欄 (必填)</t>
+  </si>
+  <si>
+    <t>C欄 (必填)</t>
+  </si>
+  <si>
+    <t>D欄 (選填)</t>
+  </si>
+  <si>
+    <t>MaterialCode</t>
+  </si>
+  <si>
+    <t>Steel Beam</t>
+  </si>
+  <si>
+    <t>MAT-2025-01</t>
+  </si>
+  <si>
+    <t>Cement</t>
+  </si>
+  <si>
+    <t>MAT-2025-02</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -68,6 +92,19 @@
       <charset val="136"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF1F1F1F"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF1F1F1F"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -77,12 +114,27 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -91,9 +143,15 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -409,26 +467,68 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F5F83F9-9D48-4AFC-B4A8-81F22523635C}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.625" defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
+    </row>
+    <row r="3" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="2">
+        <v>100</v>
+      </c>
+      <c r="D3" s="2">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="2">
+        <v>50</v>
+      </c>
+      <c r="D4" s="2">
+        <v>2000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix: Resolve Excel upload issues and extend date fields for SR/PO
</commit_message>
<xml_diff>
--- a/public/template.xlsx
+++ b/public/template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SupplyEase\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F5C1D3A-8481-4094-AA7E-ED58E2E2AF5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A59DE1A-5FB9-4665-B8DB-326560B44194}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{3B32CD19-E252-4F93-8F09-25E85353E804}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Item</t>
   </si>
@@ -43,18 +43,6 @@
   </si>
   <si>
     <t>Budget</t>
-  </si>
-  <si>
-    <t>A欄 (必填)</t>
-  </si>
-  <si>
-    <t>B欄 (必填)</t>
-  </si>
-  <si>
-    <t>C欄 (必填)</t>
-  </si>
-  <si>
-    <t>D欄 (選填)</t>
   </si>
   <si>
     <t>MaterialCode</t>
@@ -106,12 +94,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -147,10 +141,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
@@ -467,67 +461,53 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F5F83F9-9D48-4AFC-B4A8-81F22523635C}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="C11" sqref="C11:C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.625" defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>2</v>
+      <c r="C2" s="1">
+        <v>100</v>
+      </c>
+      <c r="D2" s="1">
+        <v>5000</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="2">
-        <v>100</v>
-      </c>
-      <c r="D3" s="2">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="2">
+      <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="1">
         <v>50</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D3" s="1">
         <v>2000</v>
       </c>
     </row>

</xml_diff>